<commit_message>
Activities updated for 2022
</commit_message>
<xml_diff>
--- a/data/Book1.xlsx
+++ b/data/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ueanorwich-my.sharepoint.com/personal/hpd08ucu_uea_ac_uk/Documents/CV/PL_CV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F4FD1C8-CC4F-4996-9A72-6D3ADE44B66B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{7F4FD1C8-CC4F-4996-9A72-6D3ADE44B66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F4268BB-865C-4B24-B912-F926442612CD}"/>
   <bookViews>
-    <workbookView xWindow="35100" yWindow="-585" windowWidth="21795" windowHeight="13425" xr2:uid="{7FDBA7D6-3115-46E6-B86E-F99F27BAEBAB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7FDBA7D6-3115-46E6-B86E-F99F27BAEBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,10 +450,14 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F7"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">

</xml_diff>